<commit_message>
Adding Exception message display
</commit_message>
<xml_diff>
--- a/combine_same_prefix_column_test.xlsx
+++ b/combine_same_prefix_column_test.xlsx
@@ -9,6 +9,12 @@
     <sheet name="test_data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="test_總公司" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="輸出" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="輸出1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="輸出2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="輸出3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="輸出4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="輸出5" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="輸出6" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -773,4 +779,634 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>總公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>銷貨收入</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>營業利益</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>應收帳款</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cde</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>181</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6562.234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>